<commit_message>
Remarks : file updated with tc no - 11,17,29
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_Search options.xlsx
+++ b/TCS_NEWUI_Search options.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sumit Rana\Projects\AdIntel- New\Test Cases\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E838C7C-23DB-40BF-8A59-FB6AAB9FFE6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4506"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{24948BE7-F44E-4BEA-9AF7-F64248DC213F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="4" r:id="rId1"/>
@@ -46,9 +40,9 @@
     <definedName name="test" localSheetId="1">#REF!</definedName>
     <definedName name="test">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -62,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="261">
   <si>
     <t>US#</t>
   </si>
@@ -539,38 +533,6 @@
     <t>Verify the day option above the Calendar</t>
   </si>
   <si>
-    <t>1. The Custom range should be selected
-2. User should be able to select day wise range from the Calendar</t>
-  </si>
-  <si>
-    <t>Verify the Week option above the Calendar</t>
-  </si>
-  <si>
-    <t>1. The Custom range should be selected
-2. User should be able to select Weekly date range from the Calendar</t>
-  </si>
-  <si>
-    <t>Verify the Monthly option above the Calendar</t>
-  </si>
-  <si>
-    <t>1. The Custom range should be selected
-2. User should be able to select date range Monthly from the Calendar</t>
-  </si>
-  <si>
-    <t>Verify the Quarter option above the Calendar</t>
-  </si>
-  <si>
-    <t>1. The Custom range should be selected
-2. User should be able to select date range in Quarters from the Calendar</t>
-  </si>
-  <si>
-    <t>Verify the Yearly option above the Calendar</t>
-  </si>
-  <si>
-    <t>1. The Custom range should be selected
-2. User should be able to select date range Yearly from the Calendar</t>
-  </si>
-  <si>
     <t>Verify Ad Status Search Option in All tabs as well as in its individual tab</t>
   </si>
   <si>
@@ -578,9 +540,6 @@
   </si>
   <si>
     <t>Verify Default options in Date Range search option in All Fields tab as well as in its individual tab</t>
-  </si>
-  <si>
-    <t>Verify it in both All fields tab as well as its individual tab</t>
   </si>
   <si>
     <t>Verify the Media option in All tabs and In its individual tab</t>
@@ -656,9 +615,6 @@
     <t>Click on Apply button</t>
   </si>
   <si>
-    <t>The Filters selected by the user should be applied on the report data on clicking the Apply button</t>
-  </si>
-  <si>
     <t>US:WEB-7626_TC 18</t>
   </si>
   <si>
@@ -671,13 +627,7 @@
     <t xml:space="preserve">Select Filters/options from the Search Modal </t>
   </si>
   <si>
-    <t>The options should be Selected and Reset All button should be Enabled</t>
-  </si>
-  <si>
     <t>Select Reset All button</t>
-  </si>
-  <si>
-    <t>All the options selected should be Reset to the default options</t>
   </si>
   <si>
     <t>US:WEB-7626_TC 19</t>
@@ -943,11 +893,92 @@
   <si>
     <t>US:WEB-7626_TC 13</t>
   </si>
+  <si>
+    <t>SMRT-7418,7782</t>
+  </si>
+  <si>
+    <t>As a SMART User, I want to have the ability to understand Search options functionality</t>
+  </si>
+  <si>
+    <t>TC29</t>
+  </si>
+  <si>
+    <t>Click on Week option above the Calendar</t>
+  </si>
+  <si>
+    <t>Click on Month option above the Calendar</t>
+  </si>
+  <si>
+    <t>Click on Quarter option above the Calendar</t>
+  </si>
+  <si>
+    <t>Click on Year option above the Calendar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Day option should be default selected
+2. User can select days from date range </t>
+  </si>
+  <si>
+    <t>1. The Custom range should be selected
+2. User can select only weeks from the Calendar (cant select days)</t>
+  </si>
+  <si>
+    <t>1. The Custom range should be selected
+2. Month should be displayed on Calendar
+3.  User can select only Months from the Calendar (cant select days)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The Custom range should be selected
+2. Year should be displayed on Calendar
+3. User can select only Year from the Calendar (cant select days or week)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The Custom range should be selected
+2. Quarters should be displayed on Calendar
+3. User can select only Quarters from the Calendar (cant select days or week)
+</t>
+  </si>
+  <si>
+    <t>1.The options should be Selected and Reset All button should be Enabled
+2. Also change day option to Year in Date range</t>
+  </si>
+  <si>
+    <t>1.All the options selected should be Reset to the default options
+2. Also in Date range selected "Year" option should be Reset to "Day"</t>
+  </si>
+  <si>
+    <t>SMRT-8046</t>
+  </si>
+  <si>
+    <t>Verify Search options pop up window should not close while click outside of pop up</t>
+  </si>
+  <si>
+    <t>US:WEB-7626_TC 29</t>
+  </si>
+  <si>
+    <t>Click on Search options button at the bottom right corner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search options Modal window should open with All fields as per the Account and Report selected
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on outside of pop up </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search options Modal window should not be closed
+</t>
+  </si>
+  <si>
+    <t>1. The Filters selected by the user should be applied on the report 
+2. Search options Modal window should be closed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -1869,14 +1900,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="15" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1888,6 +1919,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1895,15 +1935,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="16" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="23" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="24" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="25" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1925,23 +1956,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="40% - Accent2 2 3 2 2" xfId="15" xr:uid="{7C4AE2F6-F48E-4C74-93E8-446EE44EE508}"/>
-    <cellStyle name="Accent1 2 2 2 2 3" xfId="13" xr:uid="{893B095B-013D-4506-9986-F452B12B920C}"/>
-    <cellStyle name="Accent1 2 3 2 2" xfId="11" xr:uid="{D1A2771F-60C6-4240-82E8-8E6319A54DAD}"/>
-    <cellStyle name="Accent2 2 3 2 2" xfId="1" xr:uid="{3D7AE56F-34CD-400E-BA6D-AAD3FE78D427}"/>
-    <cellStyle name="Comma [0] 2" xfId="8" xr:uid="{C70FAD4A-663A-41D6-AE2D-00B9A7E053BA}"/>
-    <cellStyle name="Comma [0] 3" xfId="9" xr:uid="{DAFC68C9-0E88-41BD-8826-C06BF4B921BC}"/>
-    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="14" xr:uid="{0A7E0993-A444-4FFB-AE83-3A5FC57A2A5C}"/>
+    <cellStyle name="40% - Accent2 2 3 2 2" xfId="15"/>
+    <cellStyle name="Accent1 2 2 2 2 3" xfId="13"/>
+    <cellStyle name="Accent1 2 3 2 2" xfId="11"/>
+    <cellStyle name="Accent2 2 3 2 2" xfId="1"/>
+    <cellStyle name="Comma [0] 2" xfId="8"/>
+    <cellStyle name="Comma [0] 3" xfId="9"/>
+    <cellStyle name="Heading 2 2 2 2 2 3 2" xfId="14"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="12" xr:uid="{02427379-CB55-42C2-89FF-DC3A1BDF1C21}"/>
+    <cellStyle name="Hyperlink 2" xfId="12"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{DBEDEAC3-54AB-4BBF-8F7E-9ADB46A21807}"/>
-    <cellStyle name="Normal 2 4 2" xfId="10" xr:uid="{6586DCAB-C97B-4AD0-A782-9C9485892767}"/>
-    <cellStyle name="Normal 3 2 4 2" xfId="6" xr:uid="{C409EDF2-89BE-4DFC-9549-D06D48CE72AA}"/>
-    <cellStyle name="Normal 3 2 4 3" xfId="2" xr:uid="{1340F9CF-6385-4793-9938-CD0A22337B2A}"/>
-    <cellStyle name="Normal 3 2 4 3 2" xfId="4" xr:uid="{EF6168A4-6D6D-4F85-9925-6C04400B98C1}"/>
-    <cellStyle name="TableStyleLight1 3 4 2" xfId="7" xr:uid="{7DE28270-B33D-4ED8-8029-DE32734B8E04}"/>
-    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="5" xr:uid="{BB2F8CE1-CC9E-48BC-8A0B-B6BDCF9F4F66}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2 4 2" xfId="10"/>
+    <cellStyle name="Normal 3 2 4 2" xfId="6"/>
+    <cellStyle name="Normal 3 2 4 3" xfId="2"/>
+    <cellStyle name="Normal 3 2 4 3 2" xfId="4"/>
+    <cellStyle name="TableStyleLight1 3 4 2" xfId="7"/>
+    <cellStyle name="TableStyleLight1 3 4 3 2" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1957,18 +1988,10 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="148"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="48"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="48"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1991,25 +2014,22 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.3923741222529194E-2"/>
-          <c:y val="0.1418565099457787"/>
+          <c:x val="5.3923741222529187E-2"/>
+          <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321821"/>
+          <c:h val="0.75521895211321877"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2024,11 +2044,8 @@
               <a:bevelT w="63500" h="25400"/>
             </a:sp3d>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2045,7 +2062,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-3CC7-4C87-93CA-4A96F7B6D1FA}"/>
               </c:ext>
@@ -2053,8 +2070,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="E22B00"/>
@@ -2069,7 +2084,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-3CC7-4C87-93CA-4A96F7B6D1FA}"/>
               </c:ext>
@@ -2077,8 +2092,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -2093,7 +2106,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-3CC7-4C87-93CA-4A96F7B6D1FA}"/>
               </c:ext>
@@ -2101,8 +2114,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -2117,7 +2128,7 @@
                 <a:bevelT w="63500" h="25400"/>
               </a:sp3d>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-3CC7-4C87-93CA-4A96F7B6D1FA}"/>
               </c:ext>
@@ -2141,14 +2152,8 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2181,7 +2186,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2195,34 +2200,22 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-3CC7-4C87-93CA-4A96F7B6D1FA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="1420334192"/>
-        <c:axId val="1420343440"/>
+        <c:axId val="48867968"/>
+        <c:axId val="48886144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1420334192"/>
+        <c:axId val="48867968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2236,32 +2229,28 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1420343440"/>
+        <c:crossAx val="48886144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1420343440"/>
+        <c:axId val="48886144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1420334192"/>
+        <c:tickLblPos val="none"/>
+        <c:crossAx val="48867968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:effectLst/>
@@ -2275,25 +2264,17 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="145"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="45"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="45"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2316,24 +2297,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="30"/>
       <c:rotY val="32"/>
-      <c:rAngAx val="0"/>
       <c:perspective val="90"/>
     </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-    </c:backWall>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2341,9 +2310,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603381"/>
-          <c:w val="0.92496729254319687"/>
-          <c:h val="0.69766331701963358"/>
+          <c:y val="0.14624350369603398"/>
+          <c:w val="0.92496729254319798"/>
+          <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
       <c:pie3DChart>
@@ -2353,7 +2322,6 @@
           <c:order val="0"/>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3">
@@ -2362,7 +2330,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-1F1A-43A2-A67F-9D43FBDDFA5E}"/>
               </c:ext>
@@ -2370,7 +2338,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:explosion val="19"/>
             <c:spPr>
               <a:solidFill>
@@ -2380,7 +2347,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-1F1A-43A2-A67F-9D43FBDDFA5E}"/>
               </c:ext>
@@ -2404,17 +2371,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000001-1F1A-43A2-A67F-9D43FBDDFA5E}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -2433,17 +2389,6 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="1"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-1F1A-43A2-A67F-9D43FBDDFA5E}"/>
-                </c:ext>
-              </c:extLst>
             </c:dLbl>
             <c:spPr>
               <a:noFill/>
@@ -2452,14 +2397,9 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
             <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -2492,20 +2432,14 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-1F1A-43A2-A67F-9D43FBDDFA5E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
           <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
         </c:dLbls>
       </c:pie3DChart>
       <c:spPr>
@@ -2521,16 +2455,14 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253508"/>
-          <c:w val="0.42791036796598075"/>
+          <c:y val="0.88141746683253441"/>
+          <c:w val="0.42791036796598148"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln w="0"/>
@@ -2544,7 +2476,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2552,20 +2484,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2573,9 +2494,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686355E-2"/>
-          <c:w val="0.29672375522792593"/>
-          <c:h val="0.85466509216403797"/>
+          <c:y val="7.1365887012686424E-2"/>
+          <c:w val="0.29672375522792621"/>
+          <c:h val="0.85466509216403885"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -2590,7 +2511,6 @@
           </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="92D050"/>
@@ -2599,7 +2519,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0173-4321-8CAC-88CA7EFFE04D}"/>
               </c:ext>
@@ -2607,7 +2527,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -2616,7 +2535,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0173-4321-8CAC-88CA7EFFE04D}"/>
               </c:ext>
@@ -2624,7 +2543,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="FFC000"/>
@@ -2633,7 +2551,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-0173-4321-8CAC-88CA7EFFE04D}"/>
               </c:ext>
@@ -2641,7 +2559,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:srgbClr val="00B0F0"/>
@@ -2650,7 +2567,7 @@
                 <a:noFill/>
               </a:ln>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-0173-4321-8CAC-88CA7EFFE04D}"/>
               </c:ext>
@@ -2683,7 +2600,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -2697,21 +2614,12 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-0173-4321-8CAC-88CA7EFFE04D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
         <c:firstSliceAng val="0"/>
       </c:pieChart>
       <c:spPr>
@@ -2792,13 +2700,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72165251246917395"/>
-          <c:y val="3.608395161789857E-3"/>
+          <c:x val="0.72165251246917539"/>
+          <c:y val="3.6083951617898605E-3"/>
           <c:w val="0.24112408909611374"/>
-          <c:h val="0.95693837006674265"/>
+          <c:h val="0.95693837006674254"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln w="25400">
@@ -2825,7 +2732,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2857,7 +2763,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2883,7 +2789,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93F95FA3-3A9A-4305-AFFA-52E4BAA24C0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{93F95FA3-3A9A-4305-AFFA-52E4BAA24C0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2921,7 +2827,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9531D562-F1AE-493E-B6CF-CF69549BAA21}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9531D562-F1AE-493E-B6CF-CF69549BAA21}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2959,7 +2865,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D08B4E06-2AF6-4DF7-B7CF-932CD9795B3D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D08B4E06-2AF6-4DF7-B7CF-932CD9795B3D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2968,10 +2874,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2991,7 +2897,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3063,7 +2969,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB7E65A0-4003-44F1-85A9-FCE7EDFBA4CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BB7E65A0-4003-44F1-85A9-FCE7EDFBA4CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3197,7 +3103,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3247,7 +3153,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E36E588-14AD-46D7-8AF0-1D090F285222}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8E36E588-14AD-46D7-8AF0-1D090F285222}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3313,7 +3219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3365,7 +3271,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3559,14 +3465,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAFA064-7398-45ED-96EF-9A16F2B9BCC0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A5:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3630,11 +3536,11 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickTop="1">
       <c r="A8" s="67" t="s">
-        <v>235</v>
+        <v>222</v>
       </c>
       <c r="B8" s="61">
         <f>'Search Options'!C11</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8" s="61">
         <f>'Search Options'!C12</f>
@@ -3650,7 +3556,7 @@
       </c>
       <c r="F8" s="61">
         <f>SUM(B8:E8)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G8" s="62">
         <f>(B8+C8+D8)/(F8)</f>
@@ -3672,7 +3578,7 @@
       </c>
       <c r="B10" s="64">
         <f>SUM(B8:B9)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="64">
         <f>SUM(C8:C9)</f>
@@ -3688,7 +3594,7 @@
       </c>
       <c r="F10" s="64">
         <f>SUM(F8:F9)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G10" s="65">
         <f>SUM(G8:G8)</f>
@@ -3712,7 +3618,7 @@
     <mergeCell ref="G6:G7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A8" location="'Search Options'!A1" display="Redesign - Search Options" xr:uid="{2003B564-8942-4798-AC47-C1DEB0BBE807}"/>
+    <hyperlink ref="A8" location="'Search Options'!A1" display="Redesign - Search Options"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3721,20 +3627,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9155B8-21C3-4827-981C-960CD77825B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
+    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="45.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" style="10" customWidth="1"/>
     <col min="3" max="3" width="127.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.28515625" style="2" customWidth="1"/>
-    <col min="5" max="256" width="9" style="2"/>
+    <col min="4" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21" style="2" customWidth="1"/>
+    <col min="6" max="256" width="9" style="2"/>
     <col min="257" max="257" width="71.85546875" style="2" customWidth="1"/>
     <col min="258" max="258" width="18.5703125" style="2" customWidth="1"/>
     <col min="259" max="259" width="94.85546875" style="2" customWidth="1"/>
@@ -4001,7 +3906,9 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="77"/>
+      <c r="A2" s="77" t="s">
+        <v>240</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -4116,7 +4023,9 @@
       <c r="C12" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="77"/>
@@ -4176,7 +4085,7 @@
       <c r="B18" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="68" t="s">
         <v>93</v>
       </c>
       <c r="D18" s="4"/>
@@ -4264,7 +4173,7 @@
         <v>113</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="E26" s="5"/>
     </row>
@@ -4300,12 +4209,19 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="77"/>
-      <c r="B30" s="11"/>
+      <c r="B30" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>253</v>
+      </c>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="77"/>
-      <c r="B31" s="11"/>
       <c r="D31" s="4"/>
       <c r="E31" s="5"/>
     </row>
@@ -4587,10 +4503,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09530D8C-EE5E-45D3-A756-1F9B43DB51AF}">
-  <dimension ref="A1:H963"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H962"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
@@ -5328,7 +5246,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="24">
-        <v>43818</v>
+        <v>43999</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="15"/>
@@ -5336,8 +5254,8 @@
         <v>30</v>
       </c>
       <c r="G7" s="26">
-        <f>COUNTIF(G11:G1089,"Pass")</f>
-        <v>27</v>
+        <f>COUNTIF(G11:G1088,"Pass")</f>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
@@ -5352,7 +5270,7 @@
         <v>32</v>
       </c>
       <c r="G8" s="26">
-        <f>COUNTIF(G12:G1090,"Fail")</f>
+        <f>COUNTIF(G12:G1089,"Fail")</f>
         <v>1</v>
       </c>
     </row>
@@ -5370,7 +5288,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="26">
-        <f>COUNTIF(G13:G1091,"Blocked")</f>
+        <f>COUNTIF(G13:G1090,"Blocked")</f>
         <v>0</v>
       </c>
     </row>
@@ -5386,7 +5304,7 @@
         <v>37</v>
       </c>
       <c r="G10" s="26">
-        <f>COUNTIF(G14:G1092,"Not Executed")</f>
+        <f>COUNTIF(G14:G1091,"Not Executed")</f>
         <v>0</v>
       </c>
     </row>
@@ -5397,7 +5315,7 @@
       </c>
       <c r="C11" s="17">
         <f>G7</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="15"/>
@@ -5463,7 +5381,7 @@
     </row>
     <row r="17" spans="1:7" s="38" customFormat="1" ht="18.75" customHeight="1">
       <c r="A17" s="95" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="B17" s="95"/>
       <c r="C17" s="95"/>
@@ -5500,14 +5418,14 @@
       <c r="A19" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="79"/>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="80"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="86"/>
     </row>
     <row r="20" spans="1:7" s="38" customFormat="1">
       <c r="A20" s="46" t="s">
@@ -5572,12 +5490,12 @@
       <c r="A23" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="88"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="88"/>
-      <c r="G23" s="89"/>
+      <c r="B23" s="78"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="80"/>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1">
       <c r="A24" s="39" t="s">
@@ -5607,14 +5525,14 @@
       <c r="A25" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="78" t="s">
+      <c r="B25" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="80"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="86"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1">
       <c r="A26" s="46" t="s">
@@ -5681,7 +5599,7 @@
         <v>128</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D29" s="50"/>
       <c r="E29" s="51"/>
@@ -5695,10 +5613,10 @@
         <v>4</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="D30" s="50"/>
       <c r="E30" s="51"/>
@@ -5711,12 +5629,12 @@
       <c r="A31" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="87"/>
-      <c r="C31" s="88"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="89"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="80"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1">
       <c r="A32" s="39" t="s">
@@ -5746,14 +5664,14 @@
       <c r="A33" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="80"/>
+      <c r="C33" s="85"/>
+      <c r="D33" s="85"/>
+      <c r="E33" s="85"/>
+      <c r="F33" s="85"/>
+      <c r="G33" s="86"/>
     </row>
     <row r="34" spans="1:7" s="8" customFormat="1">
       <c r="A34" s="46" t="s">
@@ -5820,7 +5738,7 @@
         <v>130</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="D37" s="49"/>
       <c r="E37" s="49"/>
@@ -5833,12 +5751,12 @@
       <c r="A38" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="87"/>
-      <c r="C38" s="88"/>
-      <c r="D38" s="88"/>
-      <c r="E38" s="88"/>
-      <c r="F38" s="88"/>
-      <c r="G38" s="89"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="79"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="80"/>
     </row>
     <row r="39" spans="1:7" s="8" customFormat="1" ht="36" customHeight="1">
       <c r="A39" s="39" t="s">
@@ -5862,14 +5780,14 @@
       <c r="A40" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B40" s="78" t="s">
-        <v>237</v>
-      </c>
-      <c r="C40" s="79"/>
-      <c r="D40" s="79"/>
-      <c r="E40" s="79"/>
-      <c r="F40" s="79"/>
-      <c r="G40" s="80"/>
+      <c r="B40" s="84" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="85"/>
+      <c r="D40" s="85"/>
+      <c r="E40" s="85"/>
+      <c r="F40" s="85"/>
+      <c r="G40" s="86"/>
     </row>
     <row r="41" spans="1:7" s="8" customFormat="1">
       <c r="A41" s="46" t="s">
@@ -5949,12 +5867,12 @@
       <c r="A45" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="87"/>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="89"/>
+      <c r="B45" s="78"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="80"/>
     </row>
     <row r="46" spans="1:7" s="8" customFormat="1">
       <c r="A46" s="39" t="s">
@@ -5984,14 +5902,14 @@
       <c r="A47" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B47" s="84" t="s">
+      <c r="B47" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="85"/>
-      <c r="D47" s="85"/>
-      <c r="E47" s="85"/>
-      <c r="F47" s="85"/>
-      <c r="G47" s="86"/>
+      <c r="C47" s="88"/>
+      <c r="D47" s="88"/>
+      <c r="E47" s="88"/>
+      <c r="F47" s="88"/>
+      <c r="G47" s="89"/>
     </row>
     <row r="48" spans="1:7" s="8" customFormat="1">
       <c r="A48" s="46" t="s">
@@ -6054,12 +5972,12 @@
       <c r="A51" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B51" s="87"/>
-      <c r="C51" s="88"/>
-      <c r="D51" s="88"/>
-      <c r="E51" s="88"/>
-      <c r="F51" s="88"/>
-      <c r="G51" s="89"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="80"/>
     </row>
     <row r="52" spans="1:7" s="8" customFormat="1">
       <c r="A52" s="39" t="s">
@@ -6089,14 +6007,14 @@
       <c r="A53" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B53" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="79"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="79"/>
-      <c r="F53" s="79"/>
-      <c r="G53" s="80"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="86"/>
     </row>
     <row r="54" spans="1:7" s="8" customFormat="1">
       <c r="A54" s="46" t="s">
@@ -6159,12 +6077,12 @@
       <c r="A57" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="87"/>
-      <c r="C57" s="88"/>
-      <c r="D57" s="88"/>
-      <c r="E57" s="88"/>
-      <c r="F57" s="88"/>
-      <c r="G57" s="89"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="79"/>
+      <c r="F57" s="79"/>
+      <c r="G57" s="80"/>
     </row>
     <row r="58" spans="1:7" s="8" customFormat="1">
       <c r="A58" s="39" t="s">
@@ -6194,14 +6112,14 @@
       <c r="A59" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B59" s="84" t="s">
+      <c r="B59" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="85"/>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="86"/>
+      <c r="C59" s="88"/>
+      <c r="D59" s="88"/>
+      <c r="E59" s="88"/>
+      <c r="F59" s="88"/>
+      <c r="G59" s="89"/>
     </row>
     <row r="60" spans="1:7" s="8" customFormat="1">
       <c r="A60" s="46" t="s">
@@ -6265,10 +6183,10 @@
         <v>3</v>
       </c>
       <c r="B63" s="48" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C63" s="49" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="D63" s="49"/>
       <c r="E63" s="49"/>
@@ -6298,12 +6216,12 @@
       <c r="A65" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="87"/>
-      <c r="C65" s="88"/>
-      <c r="D65" s="88"/>
-      <c r="E65" s="88"/>
-      <c r="F65" s="88"/>
-      <c r="G65" s="89"/>
+      <c r="B65" s="78"/>
+      <c r="C65" s="79"/>
+      <c r="D65" s="79"/>
+      <c r="E65" s="79"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="80"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1">
       <c r="A66" s="39" t="s">
@@ -6333,14 +6251,14 @@
       <c r="A67" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B67" s="78" t="s">
+      <c r="B67" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="79"/>
-      <c r="D67" s="79"/>
-      <c r="E67" s="79"/>
-      <c r="F67" s="79"/>
-      <c r="G67" s="80"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="85"/>
+      <c r="E67" s="85"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="86"/>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1">
       <c r="A68" s="46" t="s">
@@ -6404,10 +6322,10 @@
         <v>3</v>
       </c>
       <c r="B71" s="48" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C71" s="49" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="D71" s="49"/>
       <c r="E71" s="49"/>
@@ -6420,12 +6338,12 @@
       <c r="A72" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="87"/>
-      <c r="C72" s="88"/>
-      <c r="D72" s="88"/>
-      <c r="E72" s="88"/>
-      <c r="F72" s="88"/>
-      <c r="G72" s="89"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="79"/>
+      <c r="D72" s="79"/>
+      <c r="E72" s="79"/>
+      <c r="F72" s="79"/>
+      <c r="G72" s="80"/>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1">
       <c r="A73" s="39" t="s">
@@ -6455,14 +6373,14 @@
       <c r="A74" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B74" s="84" t="s">
+      <c r="B74" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="C74" s="85"/>
-      <c r="D74" s="85"/>
-      <c r="E74" s="85"/>
-      <c r="F74" s="85"/>
-      <c r="G74" s="86"/>
+      <c r="C74" s="88"/>
+      <c r="D74" s="88"/>
+      <c r="E74" s="88"/>
+      <c r="F74" s="88"/>
+      <c r="G74" s="89"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A75" s="46" t="s">
@@ -6543,7 +6461,7 @@
         <v>4</v>
       </c>
       <c r="B79" s="49" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C79" s="49" t="s">
         <v>140</v>
@@ -6580,12 +6498,12 @@
       <c r="A81" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B81" s="87"/>
-      <c r="C81" s="88"/>
-      <c r="D81" s="88"/>
-      <c r="E81" s="88"/>
-      <c r="F81" s="88"/>
-      <c r="G81" s="89"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="79"/>
+      <c r="D81" s="79"/>
+      <c r="E81" s="79"/>
+      <c r="F81" s="79"/>
+      <c r="G81" s="80"/>
     </row>
     <row r="82" spans="1:7" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A82" s="39" t="s">
@@ -6615,14 +6533,14 @@
       <c r="A83" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B83" s="78" t="s">
+      <c r="B83" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C83" s="79"/>
-      <c r="D83" s="79"/>
-      <c r="E83" s="79"/>
-      <c r="F83" s="79"/>
-      <c r="G83" s="80"/>
+      <c r="C83" s="85"/>
+      <c r="D83" s="85"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="86"/>
     </row>
     <row r="84" spans="1:7" s="8" customFormat="1" ht="15.75" customHeight="1">
       <c r="A84" s="46" t="s">
@@ -6703,7 +6621,7 @@
         <v>4</v>
       </c>
       <c r="B88" s="49" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C88" s="49" t="s">
         <v>140</v>
@@ -6720,13 +6638,13 @@
         <v>5</v>
       </c>
       <c r="B89" s="49" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C89" s="49" t="s">
         <v>144</v>
       </c>
       <c r="D89" s="49" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="E89" s="49"/>
       <c r="F89" s="50" t="s">
@@ -6755,12 +6673,12 @@
       <c r="A91" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B91" s="87"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="88"/>
-      <c r="F91" s="88"/>
-      <c r="G91" s="89"/>
+      <c r="B91" s="78"/>
+      <c r="C91" s="79"/>
+      <c r="D91" s="79"/>
+      <c r="E91" s="79"/>
+      <c r="F91" s="79"/>
+      <c r="G91" s="80"/>
     </row>
     <row r="92" spans="1:7" s="8" customFormat="1" ht="17.25" customHeight="1">
       <c r="A92" s="39" t="s">
@@ -6783,21 +6701,21 @@
       </c>
       <c r="G92" s="44" t="str">
         <f>IF(COUNTIF(F95:F102,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F95:F102,"Fail")&gt;0,"Fail",IF(COUNTIF(F95:F102,"")=0,"Pass","Not Executed")))</f>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
     </row>
     <row r="93" spans="1:7" s="8" customFormat="1" ht="30" customHeight="1">
       <c r="A93" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B93" s="78" t="s">
+      <c r="B93" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C93" s="79"/>
-      <c r="D93" s="79"/>
-      <c r="E93" s="79"/>
-      <c r="F93" s="79"/>
-      <c r="G93" s="80"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="85"/>
+      <c r="E93" s="85"/>
+      <c r="F93" s="85"/>
+      <c r="G93" s="86"/>
     </row>
     <row r="94" spans="1:7" s="8" customFormat="1">
       <c r="A94" s="46" t="s">
@@ -6881,82 +6799,80 @@
         <v>147</v>
       </c>
       <c r="C98" s="49" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
       <c r="D98" s="49"/>
       <c r="E98" s="49"/>
       <c r="F98" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="G98" s="51" t="s">
-        <v>160</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="G98" s="51"/>
     </row>
     <row r="99" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A99" s="47">
         <v>5</v>
       </c>
       <c r="B99" s="48" t="s">
-        <v>149</v>
+        <v>242</v>
       </c>
       <c r="C99" s="49" t="s">
-        <v>150</v>
+        <v>247</v>
       </c>
       <c r="D99" s="49"/>
       <c r="E99" s="49"/>
       <c r="F99" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G99" s="51"/>
     </row>
-    <row r="100" spans="1:8" ht="30">
+    <row r="100" spans="1:8" ht="45">
       <c r="A100" s="47">
         <v>6</v>
       </c>
       <c r="B100" s="48" t="s">
-        <v>151</v>
+        <v>243</v>
       </c>
       <c r="C100" s="49" t="s">
-        <v>152</v>
+        <v>248</v>
       </c>
       <c r="D100" s="49"/>
       <c r="E100" s="49"/>
       <c r="F100" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G100" s="51"/>
     </row>
-    <row r="101" spans="1:8" ht="30">
+    <row r="101" spans="1:8" ht="60">
       <c r="A101" s="47">
         <v>7</v>
       </c>
       <c r="B101" s="48" t="s">
-        <v>153</v>
+        <v>244</v>
       </c>
       <c r="C101" s="49" t="s">
-        <v>154</v>
+        <v>250</v>
       </c>
       <c r="D101" s="49"/>
       <c r="E101" s="49"/>
       <c r="F101" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G101" s="51"/>
     </row>
-    <row r="102" spans="1:8" ht="30">
+    <row r="102" spans="1:8" ht="60">
       <c r="A102" s="47">
         <v>8</v>
       </c>
       <c r="B102" s="48" t="s">
-        <v>155</v>
+        <v>245</v>
       </c>
       <c r="C102" s="49" t="s">
-        <v>156</v>
+        <v>249</v>
       </c>
       <c r="D102" s="49"/>
       <c r="E102" s="49"/>
       <c r="F102" s="50" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G102" s="51"/>
     </row>
@@ -6964,12 +6880,12 @@
       <c r="A103" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B103" s="87"/>
-      <c r="C103" s="88"/>
-      <c r="D103" s="88"/>
-      <c r="E103" s="88"/>
-      <c r="F103" s="88"/>
-      <c r="G103" s="89"/>
+      <c r="B103" s="78"/>
+      <c r="C103" s="79"/>
+      <c r="D103" s="79"/>
+      <c r="E103" s="79"/>
+      <c r="F103" s="79"/>
+      <c r="G103" s="80"/>
     </row>
     <row r="104" spans="1:8">
       <c r="A104" s="39" t="s">
@@ -6999,14 +6915,14 @@
       <c r="A105" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B105" s="78" t="s">
+      <c r="B105" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C105" s="79"/>
-      <c r="D105" s="79"/>
-      <c r="E105" s="79"/>
-      <c r="F105" s="79"/>
-      <c r="G105" s="80"/>
+      <c r="C105" s="85"/>
+      <c r="D105" s="85"/>
+      <c r="E105" s="85"/>
+      <c r="F105" s="85"/>
+      <c r="G105" s="86"/>
     </row>
     <row r="106" spans="1:8">
       <c r="A106" s="46" t="s">
@@ -7070,10 +6986,10 @@
         <v>3</v>
       </c>
       <c r="B109" s="48" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C109" s="49" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="D109" s="49"/>
       <c r="E109" s="49"/>
@@ -7087,10 +7003,10 @@
         <v>4</v>
       </c>
       <c r="B110" s="49" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C110" s="49" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="D110" s="49"/>
       <c r="E110" s="49"/>
@@ -7103,16 +7019,16 @@
       <c r="A111" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B111" s="87"/>
-      <c r="C111" s="88"/>
-      <c r="D111" s="88"/>
-      <c r="E111" s="88"/>
-      <c r="F111" s="88"/>
-      <c r="G111" s="89"/>
+      <c r="B111" s="78"/>
+      <c r="C111" s="79"/>
+      <c r="D111" s="79"/>
+      <c r="E111" s="79"/>
+      <c r="F111" s="79"/>
+      <c r="G111" s="80"/>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="39" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B112" s="81" t="s">
         <v>92</v>
@@ -7139,14 +7055,14 @@
       <c r="A113" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B113" s="78" t="s">
+      <c r="B113" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C113" s="79"/>
-      <c r="D113" s="79"/>
-      <c r="E113" s="79"/>
-      <c r="F113" s="79"/>
-      <c r="G113" s="80"/>
+      <c r="C113" s="85"/>
+      <c r="D113" s="85"/>
+      <c r="E113" s="85"/>
+      <c r="F113" s="85"/>
+      <c r="G113" s="86"/>
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="46" t="s">
@@ -7210,10 +7126,10 @@
         <v>3</v>
       </c>
       <c r="B117" s="48" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C117" s="49" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D117" s="49"/>
       <c r="E117" s="49"/>
@@ -7227,10 +7143,10 @@
         <v>4</v>
       </c>
       <c r="B118" s="49" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C118" s="49" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D118" s="49"/>
       <c r="E118" s="49"/>
@@ -7243,16 +7159,16 @@
       <c r="A119" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B119" s="87"/>
-      <c r="C119" s="88"/>
-      <c r="D119" s="88"/>
-      <c r="E119" s="88"/>
-      <c r="F119" s="88"/>
-      <c r="G119" s="89"/>
+      <c r="B119" s="78"/>
+      <c r="C119" s="79"/>
+      <c r="D119" s="79"/>
+      <c r="E119" s="79"/>
+      <c r="F119" s="79"/>
+      <c r="G119" s="80"/>
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="39" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B120" s="81" t="s">
         <v>81</v>
@@ -7278,14 +7194,14 @@
       <c r="A121" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B121" s="78" t="s">
+      <c r="B121" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C121" s="79"/>
-      <c r="D121" s="79"/>
-      <c r="E121" s="79"/>
-      <c r="F121" s="79"/>
-      <c r="G121" s="80"/>
+      <c r="C121" s="85"/>
+      <c r="D121" s="85"/>
+      <c r="E121" s="85"/>
+      <c r="F121" s="85"/>
+      <c r="G121" s="86"/>
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="46" t="s">
@@ -7349,10 +7265,10 @@
         <v>3</v>
       </c>
       <c r="B125" s="48" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="C125" s="49" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="D125" s="49"/>
       <c r="E125" s="49"/>
@@ -7366,13 +7282,13 @@
         <v>4</v>
       </c>
       <c r="B126" s="49" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C126" s="49" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D126" s="49" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="E126" s="49"/>
       <c r="F126" s="50" t="s">
@@ -7384,16 +7300,16 @@
       <c r="A127" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B127" s="87"/>
-      <c r="C127" s="88"/>
-      <c r="D127" s="88"/>
-      <c r="E127" s="88"/>
-      <c r="F127" s="88"/>
-      <c r="G127" s="89"/>
+      <c r="B127" s="78"/>
+      <c r="C127" s="79"/>
+      <c r="D127" s="79"/>
+      <c r="E127" s="79"/>
+      <c r="F127" s="79"/>
+      <c r="G127" s="80"/>
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="39" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B128" s="81" t="s">
         <v>82</v>
@@ -7419,14 +7335,14 @@
       <c r="A129" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B129" s="78" t="s">
+      <c r="B129" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C129" s="79"/>
-      <c r="D129" s="79"/>
-      <c r="E129" s="79"/>
-      <c r="F129" s="79"/>
-      <c r="G129" s="80"/>
+      <c r="C129" s="85"/>
+      <c r="D129" s="85"/>
+      <c r="E129" s="85"/>
+      <c r="F129" s="85"/>
+      <c r="G129" s="86"/>
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="46" t="s">
@@ -7490,10 +7406,10 @@
         <v>3</v>
       </c>
       <c r="B133" s="48" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="C133" s="49" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D133" s="49"/>
       <c r="E133" s="49"/>
@@ -7507,10 +7423,10 @@
         <v>4</v>
       </c>
       <c r="B134" s="49" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="C134" s="49" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="D134" s="49"/>
       <c r="E134" s="49"/>
@@ -7523,16 +7439,16 @@
       <c r="A135" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B135" s="87"/>
-      <c r="C135" s="88"/>
-      <c r="D135" s="88"/>
-      <c r="E135" s="88"/>
-      <c r="F135" s="88"/>
-      <c r="G135" s="89"/>
+      <c r="B135" s="78"/>
+      <c r="C135" s="79"/>
+      <c r="D135" s="79"/>
+      <c r="E135" s="79"/>
+      <c r="F135" s="79"/>
+      <c r="G135" s="80"/>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="39" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B136" s="81" t="s">
         <v>83</v>
@@ -7558,14 +7474,14 @@
       <c r="A137" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B137" s="78" t="s">
+      <c r="B137" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C137" s="79"/>
-      <c r="D137" s="79"/>
-      <c r="E137" s="79"/>
-      <c r="F137" s="79"/>
-      <c r="G137" s="80"/>
+      <c r="C137" s="85"/>
+      <c r="D137" s="85"/>
+      <c r="E137" s="85"/>
+      <c r="F137" s="85"/>
+      <c r="G137" s="86"/>
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="46" t="s">
@@ -7629,10 +7545,10 @@
         <v>3</v>
       </c>
       <c r="B141" s="48" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C141" s="49" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="D141" s="49"/>
       <c r="E141" s="49"/>
@@ -7646,10 +7562,10 @@
         <v>4</v>
       </c>
       <c r="B142" s="49" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C142" s="49" t="s">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="D142" s="49"/>
       <c r="E142" s="49"/>
@@ -7662,16 +7578,16 @@
       <c r="A143" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B143" s="87"/>
-      <c r="C143" s="88"/>
-      <c r="D143" s="88"/>
-      <c r="E143" s="88"/>
-      <c r="F143" s="88"/>
-      <c r="G143" s="89"/>
+      <c r="B143" s="78"/>
+      <c r="C143" s="79"/>
+      <c r="D143" s="79"/>
+      <c r="E143" s="79"/>
+      <c r="F143" s="79"/>
+      <c r="G143" s="80"/>
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="39" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B144" s="81" t="s">
         <v>93</v>
@@ -7697,14 +7613,14 @@
       <c r="A145" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B145" s="78" t="s">
+      <c r="B145" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C145" s="79"/>
-      <c r="D145" s="79"/>
-      <c r="E145" s="79"/>
-      <c r="F145" s="79"/>
-      <c r="G145" s="80"/>
+      <c r="C145" s="85"/>
+      <c r="D145" s="85"/>
+      <c r="E145" s="85"/>
+      <c r="F145" s="85"/>
+      <c r="G145" s="86"/>
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="46" t="s">
@@ -7768,10 +7684,10 @@
         <v>3</v>
       </c>
       <c r="B149" s="48" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C149" s="49" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D149" s="49"/>
       <c r="E149" s="49"/>
@@ -7780,15 +7696,15 @@
       </c>
       <c r="G149" s="51"/>
     </row>
-    <row r="150" spans="1:7" ht="15.75">
+    <row r="150" spans="1:7" ht="30">
       <c r="A150" s="47">
         <v>4</v>
       </c>
       <c r="B150" s="49" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C150" s="49" t="s">
-        <v>186</v>
+        <v>251</v>
       </c>
       <c r="D150" s="49"/>
       <c r="E150" s="49"/>
@@ -7797,15 +7713,15 @@
       </c>
       <c r="G150" s="51"/>
     </row>
-    <row r="151" spans="1:7" ht="15.75">
+    <row r="151" spans="1:7" ht="30">
       <c r="A151" s="47">
         <v>5</v>
       </c>
       <c r="B151" s="49" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C151" s="49" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
       <c r="D151" s="49"/>
       <c r="E151" s="49"/>
@@ -7818,16 +7734,16 @@
       <c r="A152" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B152" s="87"/>
-      <c r="C152" s="88"/>
-      <c r="D152" s="88"/>
-      <c r="E152" s="88"/>
-      <c r="F152" s="88"/>
-      <c r="G152" s="89"/>
+      <c r="B152" s="78"/>
+      <c r="C152" s="79"/>
+      <c r="D152" s="79"/>
+      <c r="E152" s="79"/>
+      <c r="F152" s="79"/>
+      <c r="G152" s="80"/>
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="39" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="B153" s="81" t="s">
         <v>84</v>
@@ -7853,14 +7769,14 @@
       <c r="A154" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B154" s="78" t="s">
+      <c r="B154" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C154" s="79"/>
-      <c r="D154" s="79"/>
-      <c r="E154" s="79"/>
-      <c r="F154" s="79"/>
-      <c r="G154" s="80"/>
+      <c r="C154" s="85"/>
+      <c r="D154" s="85"/>
+      <c r="E154" s="85"/>
+      <c r="F154" s="85"/>
+      <c r="G154" s="86"/>
     </row>
     <row r="155" spans="1:7" ht="30.95" customHeight="1">
       <c r="A155" s="46" t="s">
@@ -7924,10 +7840,10 @@
         <v>3</v>
       </c>
       <c r="B158" s="48" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="C158" s="49" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="D158" s="49"/>
       <c r="E158" s="49"/>
@@ -7940,16 +7856,16 @@
       <c r="A159" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B159" s="87"/>
-      <c r="C159" s="88"/>
-      <c r="D159" s="88"/>
-      <c r="E159" s="88"/>
-      <c r="F159" s="88"/>
-      <c r="G159" s="89"/>
+      <c r="B159" s="78"/>
+      <c r="C159" s="79"/>
+      <c r="D159" s="79"/>
+      <c r="E159" s="79"/>
+      <c r="F159" s="79"/>
+      <c r="G159" s="80"/>
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="39" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="B160" s="81" t="s">
         <v>96</v>
@@ -7975,14 +7891,14 @@
       <c r="A161" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B161" s="78" t="s">
+      <c r="B161" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C161" s="79"/>
-      <c r="D161" s="79"/>
-      <c r="E161" s="79"/>
-      <c r="F161" s="79"/>
-      <c r="G161" s="80"/>
+      <c r="C161" s="85"/>
+      <c r="D161" s="85"/>
+      <c r="E161" s="85"/>
+      <c r="F161" s="85"/>
+      <c r="G161" s="86"/>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="46" t="s">
@@ -8046,13 +7962,13 @@
         <v>3</v>
       </c>
       <c r="B165" s="48" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C165" s="49" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="D165" s="49" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="E165" s="49"/>
       <c r="F165" s="50" t="s">
@@ -8065,10 +7981,10 @@
         <v>4</v>
       </c>
       <c r="B166" s="48" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C166" s="49" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="D166" s="49"/>
       <c r="E166" s="49"/>
@@ -8081,16 +7997,16 @@
       <c r="A167" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B167" s="87"/>
-      <c r="C167" s="88"/>
-      <c r="D167" s="88"/>
-      <c r="E167" s="88"/>
-      <c r="F167" s="88"/>
-      <c r="G167" s="89"/>
+      <c r="B167" s="78"/>
+      <c r="C167" s="79"/>
+      <c r="D167" s="79"/>
+      <c r="E167" s="79"/>
+      <c r="F167" s="79"/>
+      <c r="G167" s="80"/>
     </row>
     <row r="168" spans="1:7">
       <c r="A168" s="39" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B168" s="81" t="s">
         <v>98</v>
@@ -8116,14 +8032,14 @@
       <c r="A169" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B169" s="78" t="s">
+      <c r="B169" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C169" s="79"/>
-      <c r="D169" s="79"/>
-      <c r="E169" s="79"/>
-      <c r="F169" s="79"/>
-      <c r="G169" s="80"/>
+      <c r="C169" s="85"/>
+      <c r="D169" s="85"/>
+      <c r="E169" s="85"/>
+      <c r="F169" s="85"/>
+      <c r="G169" s="86"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="46" t="s">
@@ -8159,7 +8075,7 @@
         <v>121</v>
       </c>
       <c r="D171" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E171" s="49"/>
       <c r="F171" s="50" t="s">
@@ -8189,10 +8105,10 @@
         <v>3</v>
       </c>
       <c r="B173" s="48" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="C173" s="49" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="D173" s="49"/>
       <c r="E173" s="49"/>
@@ -8206,10 +8122,10 @@
         <v>4</v>
       </c>
       <c r="B174" s="49" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="C174" s="49" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="D174" s="49"/>
       <c r="E174" s="49"/>
@@ -8222,16 +8138,16 @@
       <c r="A175" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B175" s="87"/>
-      <c r="C175" s="88"/>
-      <c r="D175" s="88"/>
-      <c r="E175" s="88"/>
-      <c r="F175" s="88"/>
-      <c r="G175" s="89"/>
+      <c r="B175" s="78"/>
+      <c r="C175" s="79"/>
+      <c r="D175" s="79"/>
+      <c r="E175" s="79"/>
+      <c r="F175" s="79"/>
+      <c r="G175" s="80"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="39" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B176" s="81" t="s">
         <v>100</v>
@@ -8257,14 +8173,14 @@
       <c r="A177" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B177" s="78" t="s">
+      <c r="B177" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C177" s="79"/>
-      <c r="D177" s="79"/>
-      <c r="E177" s="79"/>
-      <c r="F177" s="79"/>
-      <c r="G177" s="80"/>
+      <c r="C177" s="85"/>
+      <c r="D177" s="85"/>
+      <c r="E177" s="85"/>
+      <c r="F177" s="85"/>
+      <c r="G177" s="86"/>
     </row>
     <row r="178" spans="1:7">
       <c r="A178" s="46" t="s">
@@ -8300,7 +8216,7 @@
         <v>121</v>
       </c>
       <c r="D179" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E179" s="49"/>
       <c r="F179" s="50" t="s">
@@ -8330,10 +8246,10 @@
         <v>3</v>
       </c>
       <c r="B181" s="48" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C181" s="49" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="D181" s="49"/>
       <c r="E181" s="49"/>
@@ -8347,10 +8263,10 @@
         <v>4</v>
       </c>
       <c r="B182" s="49" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="C182" s="49" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="D182" s="49"/>
       <c r="E182" s="49"/>
@@ -8363,16 +8279,16 @@
       <c r="A183" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B183" s="87"/>
-      <c r="C183" s="88"/>
-      <c r="D183" s="88"/>
-      <c r="E183" s="88"/>
-      <c r="F183" s="88"/>
-      <c r="G183" s="89"/>
+      <c r="B183" s="78"/>
+      <c r="C183" s="79"/>
+      <c r="D183" s="79"/>
+      <c r="E183" s="79"/>
+      <c r="F183" s="79"/>
+      <c r="G183" s="80"/>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="39" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B184" s="81" t="s">
         <v>101</v>
@@ -8398,14 +8314,14 @@
       <c r="A185" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B185" s="78" t="s">
+      <c r="B185" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C185" s="79"/>
-      <c r="D185" s="79"/>
-      <c r="E185" s="79"/>
-      <c r="F185" s="79"/>
-      <c r="G185" s="80"/>
+      <c r="C185" s="85"/>
+      <c r="D185" s="85"/>
+      <c r="E185" s="85"/>
+      <c r="F185" s="85"/>
+      <c r="G185" s="86"/>
     </row>
     <row r="186" spans="1:7">
       <c r="A186" s="46" t="s">
@@ -8441,7 +8357,7 @@
         <v>121</v>
       </c>
       <c r="D187" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E187" s="49"/>
       <c r="F187" s="50" t="s">
@@ -8471,10 +8387,10 @@
         <v>3</v>
       </c>
       <c r="B189" s="48" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C189" s="49" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="D189" s="49"/>
       <c r="E189" s="49"/>
@@ -8488,10 +8404,10 @@
         <v>4</v>
       </c>
       <c r="B190" s="49" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="C190" s="49" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D190" s="49"/>
       <c r="E190" s="49"/>
@@ -8504,16 +8420,16 @@
       <c r="A191" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B191" s="87"/>
-      <c r="C191" s="88"/>
-      <c r="D191" s="88"/>
-      <c r="E191" s="88"/>
-      <c r="F191" s="88"/>
-      <c r="G191" s="89"/>
+      <c r="B191" s="78"/>
+      <c r="C191" s="79"/>
+      <c r="D191" s="79"/>
+      <c r="E191" s="79"/>
+      <c r="F191" s="79"/>
+      <c r="G191" s="80"/>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" s="39" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="B192" s="81" t="s">
         <v>105</v>
@@ -8539,14 +8455,14 @@
       <c r="A193" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B193" s="78" t="s">
+      <c r="B193" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C193" s="79"/>
-      <c r="D193" s="79"/>
-      <c r="E193" s="79"/>
-      <c r="F193" s="79"/>
-      <c r="G193" s="80"/>
+      <c r="C193" s="85"/>
+      <c r="D193" s="85"/>
+      <c r="E193" s="85"/>
+      <c r="F193" s="85"/>
+      <c r="G193" s="86"/>
     </row>
     <row r="194" spans="1:7">
       <c r="A194" s="46" t="s">
@@ -8582,7 +8498,7 @@
         <v>121</v>
       </c>
       <c r="D195" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E195" s="49"/>
       <c r="F195" s="50" t="s">
@@ -8612,10 +8528,10 @@
         <v>3</v>
       </c>
       <c r="B197" s="48" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="C197" s="49" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="D197" s="49"/>
       <c r="E197" s="49"/>
@@ -8629,10 +8545,10 @@
         <v>4</v>
       </c>
       <c r="B198" s="49" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C198" s="49" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="D198" s="49"/>
       <c r="E198" s="49"/>
@@ -8645,16 +8561,16 @@
       <c r="A199" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B199" s="87"/>
-      <c r="C199" s="88"/>
-      <c r="D199" s="88"/>
-      <c r="E199" s="88"/>
-      <c r="F199" s="88"/>
-      <c r="G199" s="89"/>
+      <c r="B199" s="78"/>
+      <c r="C199" s="79"/>
+      <c r="D199" s="79"/>
+      <c r="E199" s="79"/>
+      <c r="F199" s="79"/>
+      <c r="G199" s="80"/>
     </row>
     <row r="200" spans="1:7">
       <c r="A200" s="39" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="B200" s="81" t="s">
         <v>106</v>
@@ -8680,14 +8596,14 @@
       <c r="A201" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B201" s="78" t="s">
+      <c r="B201" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C201" s="79"/>
-      <c r="D201" s="79"/>
-      <c r="E201" s="79"/>
-      <c r="F201" s="79"/>
-      <c r="G201" s="80"/>
+      <c r="C201" s="85"/>
+      <c r="D201" s="85"/>
+      <c r="E201" s="85"/>
+      <c r="F201" s="85"/>
+      <c r="G201" s="86"/>
     </row>
     <row r="202" spans="1:7">
       <c r="A202" s="46" t="s">
@@ -8723,7 +8639,7 @@
         <v>121</v>
       </c>
       <c r="D203" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E203" s="49"/>
       <c r="F203" s="50" t="s">
@@ -8753,10 +8669,10 @@
         <v>3</v>
       </c>
       <c r="B205" s="48" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="C205" s="49" t="s">
-        <v>224</v>
+        <v>211</v>
       </c>
       <c r="D205" s="49"/>
       <c r="E205" s="49"/>
@@ -8770,10 +8686,10 @@
         <v>4</v>
       </c>
       <c r="B206" s="49" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C206" s="49" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D206" s="49"/>
       <c r="E206" s="49"/>
@@ -8786,19 +8702,19 @@
       <c r="A207" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B207" s="87"/>
-      <c r="C207" s="88"/>
-      <c r="D207" s="88"/>
-      <c r="E207" s="88"/>
-      <c r="F207" s="88"/>
-      <c r="G207" s="89"/>
+      <c r="B207" s="78"/>
+      <c r="C207" s="79"/>
+      <c r="D207" s="79"/>
+      <c r="E207" s="79"/>
+      <c r="F207" s="79"/>
+      <c r="G207" s="80"/>
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="39" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="B208" s="81" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="C208" s="82" t="s">
         <v>107</v>
@@ -8821,14 +8737,14 @@
       <c r="A209" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B209" s="78" t="s">
+      <c r="B209" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C209" s="79"/>
-      <c r="D209" s="79"/>
-      <c r="E209" s="79"/>
-      <c r="F209" s="79"/>
-      <c r="G209" s="80"/>
+      <c r="C209" s="85"/>
+      <c r="D209" s="85"/>
+      <c r="E209" s="85"/>
+      <c r="F209" s="85"/>
+      <c r="G209" s="86"/>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="46" t="s">
@@ -8864,7 +8780,7 @@
         <v>121</v>
       </c>
       <c r="D211" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E211" s="49"/>
       <c r="F211" s="50" t="s">
@@ -8894,10 +8810,10 @@
         <v>3</v>
       </c>
       <c r="B213" s="48" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C213" s="49" t="s">
-        <v>225</v>
+        <v>212</v>
       </c>
       <c r="D213" s="49"/>
       <c r="E213" s="49"/>
@@ -8911,10 +8827,10 @@
         <v>4</v>
       </c>
       <c r="B214" s="49" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C214" s="49" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D214" s="49"/>
       <c r="E214" s="49"/>
@@ -8927,16 +8843,16 @@
       <c r="A215" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B215" s="87"/>
-      <c r="C215" s="88"/>
-      <c r="D215" s="88"/>
-      <c r="E215" s="88"/>
-      <c r="F215" s="88"/>
-      <c r="G215" s="89"/>
+      <c r="B215" s="78"/>
+      <c r="C215" s="79"/>
+      <c r="D215" s="79"/>
+      <c r="E215" s="79"/>
+      <c r="F215" s="79"/>
+      <c r="G215" s="80"/>
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="39" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="B216" s="81" t="s">
         <v>108</v>
@@ -8962,14 +8878,14 @@
       <c r="A217" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B217" s="78" t="s">
+      <c r="B217" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C217" s="79"/>
-      <c r="D217" s="79"/>
-      <c r="E217" s="79"/>
-      <c r="F217" s="79"/>
-      <c r="G217" s="80"/>
+      <c r="C217" s="85"/>
+      <c r="D217" s="85"/>
+      <c r="E217" s="85"/>
+      <c r="F217" s="85"/>
+      <c r="G217" s="86"/>
     </row>
     <row r="218" spans="1:7">
       <c r="A218" s="46" t="s">
@@ -9005,7 +8921,7 @@
         <v>121</v>
       </c>
       <c r="D219" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E219" s="49"/>
       <c r="F219" s="50" t="s">
@@ -9035,10 +8951,10 @@
         <v>3</v>
       </c>
       <c r="B221" s="48" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="C221" s="49" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D221" s="49"/>
       <c r="E221" s="49"/>
@@ -9052,10 +8968,10 @@
         <v>4</v>
       </c>
       <c r="B222" s="49" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C222" s="49" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D222" s="49"/>
       <c r="E222" s="49"/>
@@ -9068,16 +8984,16 @@
       <c r="A223" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B223" s="87"/>
-      <c r="C223" s="88"/>
-      <c r="D223" s="88"/>
-      <c r="E223" s="88"/>
-      <c r="F223" s="88"/>
-      <c r="G223" s="89"/>
+      <c r="B223" s="78"/>
+      <c r="C223" s="79"/>
+      <c r="D223" s="79"/>
+      <c r="E223" s="79"/>
+      <c r="F223" s="79"/>
+      <c r="G223" s="80"/>
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="39" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="B224" s="81" t="s">
         <v>109</v>
@@ -9103,14 +9019,14 @@
       <c r="A225" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B225" s="78" t="s">
+      <c r="B225" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C225" s="79"/>
-      <c r="D225" s="79"/>
-      <c r="E225" s="79"/>
-      <c r="F225" s="79"/>
-      <c r="G225" s="80"/>
+      <c r="C225" s="85"/>
+      <c r="D225" s="85"/>
+      <c r="E225" s="85"/>
+      <c r="F225" s="85"/>
+      <c r="G225" s="86"/>
     </row>
     <row r="226" spans="1:7">
       <c r="A226" s="46" t="s">
@@ -9146,7 +9062,7 @@
         <v>121</v>
       </c>
       <c r="D227" s="49" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E227" s="49"/>
       <c r="F227" s="50" t="s">
@@ -9176,10 +9092,10 @@
         <v>3</v>
       </c>
       <c r="B229" s="48" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="C229" s="49" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="D229" s="49"/>
       <c r="E229" s="49"/>
@@ -9193,10 +9109,10 @@
         <v>4</v>
       </c>
       <c r="B230" s="49" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="C230" s="49" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="D230" s="49"/>
       <c r="E230" s="49"/>
@@ -9209,16 +9125,16 @@
       <c r="A231" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B231" s="87"/>
-      <c r="C231" s="88"/>
-      <c r="D231" s="88"/>
-      <c r="E231" s="88"/>
-      <c r="F231" s="88"/>
-      <c r="G231" s="89"/>
+      <c r="B231" s="78"/>
+      <c r="C231" s="79"/>
+      <c r="D231" s="79"/>
+      <c r="E231" s="79"/>
+      <c r="F231" s="79"/>
+      <c r="G231" s="80"/>
     </row>
     <row r="232" spans="1:7">
       <c r="A232" s="39" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="B232" s="81" t="s">
         <v>115</v>
@@ -9244,14 +9160,14 @@
       <c r="A233" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B233" s="78" t="s">
+      <c r="B233" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C233" s="79"/>
-      <c r="D233" s="79"/>
-      <c r="E233" s="79"/>
-      <c r="F233" s="79"/>
-      <c r="G233" s="80"/>
+      <c r="C233" s="85"/>
+      <c r="D233" s="85"/>
+      <c r="E233" s="85"/>
+      <c r="F233" s="85"/>
+      <c r="G233" s="86"/>
     </row>
     <row r="234" spans="1:7">
       <c r="A234" s="46" t="s">
@@ -9320,7 +9236,7 @@
         <v>128</v>
       </c>
       <c r="C237" s="49" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="D237" s="49"/>
       <c r="E237" s="49"/>
@@ -9334,13 +9250,13 @@
         <v>4</v>
       </c>
       <c r="B238" s="49" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="C238" s="49" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="D238" s="49" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="E238" s="49"/>
       <c r="F238" s="50" t="s">
@@ -9352,75 +9268,136 @@
       <c r="A239" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="B239" s="87"/>
-      <c r="C239" s="88"/>
-      <c r="D239" s="88"/>
-      <c r="E239" s="88"/>
-      <c r="F239" s="88"/>
-      <c r="G239" s="89"/>
+      <c r="B239" s="78"/>
+      <c r="C239" s="79"/>
+      <c r="D239" s="79"/>
+      <c r="E239" s="79"/>
+      <c r="F239" s="79"/>
+      <c r="G239" s="80"/>
     </row>
     <row r="240" spans="1:7">
-      <c r="A240" s="8"/>
-      <c r="B240" s="8"/>
-      <c r="C240" s="8"/>
-      <c r="D240" s="8"/>
-      <c r="E240" s="8"/>
-      <c r="F240" s="8"/>
-      <c r="G240" s="8"/>
-    </row>
-    <row r="241" spans="1:7">
-      <c r="A241" s="8"/>
-      <c r="B241" s="8"/>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="8"/>
+      <c r="A240" s="39" t="s">
+        <v>255</v>
+      </c>
+      <c r="B240" s="81" t="s">
+        <v>254</v>
+      </c>
+      <c r="C240" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="D240" s="82" t="s">
+        <v>115</v>
+      </c>
+      <c r="E240" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="F240" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G240" s="44" t="str">
+        <f>IF(COUNTIF(F243:F245,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F243:F245,"Fail")&gt;0,"Fail",IF(COUNTIF(F243:F245,"")=0,"Pass","Not Executed")))</f>
+        <v>Fail</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" ht="29.25" customHeight="1">
+      <c r="A241" s="45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B241" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="C241" s="85"/>
+      <c r="D241" s="85"/>
+      <c r="E241" s="85"/>
+      <c r="F241" s="85"/>
+      <c r="G241" s="86"/>
     </row>
     <row r="242" spans="1:7">
-      <c r="A242" s="8"/>
-      <c r="B242" s="8"/>
-      <c r="C242" s="8"/>
-      <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="8"/>
-    </row>
-    <row r="243" spans="1:7">
-      <c r="A243" s="8"/>
-      <c r="B243" s="8"/>
-      <c r="C243" s="8"/>
-      <c r="D243" s="8"/>
-      <c r="E243" s="8"/>
-      <c r="F243" s="8"/>
-      <c r="G243" s="8"/>
-    </row>
-    <row r="244" spans="1:7">
-      <c r="A244" s="8"/>
-      <c r="B244" s="8"/>
-      <c r="C244" s="8"/>
-      <c r="D244" s="8"/>
-      <c r="E244" s="8"/>
-      <c r="F244" s="8"/>
-      <c r="G244" s="8"/>
-    </row>
-    <row r="245" spans="1:7">
-      <c r="A245" s="8"/>
-      <c r="B245" s="8"/>
-      <c r="C245" s="8"/>
-      <c r="D245" s="8"/>
-      <c r="E245" s="8"/>
-      <c r="F245" s="8"/>
-      <c r="G245" s="8"/>
+      <c r="A242" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B242" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C242" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D242" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="E242" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="F242" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="G242" s="46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" ht="150">
+      <c r="A243" s="47">
+        <v>1</v>
+      </c>
+      <c r="B243" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C243" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D243" s="49" t="s">
+        <v>54</v>
+      </c>
+      <c r="E243" s="49"/>
+      <c r="F243" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G243" s="51"/>
+    </row>
+    <row r="244" spans="1:7" ht="45">
+      <c r="A244" s="47">
+        <v>2</v>
+      </c>
+      <c r="B244" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="C244" s="49" t="s">
+        <v>257</v>
+      </c>
+      <c r="D244" s="49"/>
+      <c r="E244" s="49"/>
+      <c r="F244" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="G244" s="51"/>
+    </row>
+    <row r="245" spans="1:7" ht="30">
+      <c r="A245" s="47">
+        <v>3</v>
+      </c>
+      <c r="B245" s="49" t="s">
+        <v>258</v>
+      </c>
+      <c r="C245" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="D245" s="49"/>
+      <c r="E245" s="49"/>
+      <c r="F245" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="G245" s="51"/>
     </row>
     <row r="246" spans="1:7">
-      <c r="A246" s="8"/>
-      <c r="B246" s="8"/>
-      <c r="C246" s="8"/>
-      <c r="D246" s="8"/>
-      <c r="E246" s="8"/>
-      <c r="F246" s="8"/>
-      <c r="G246" s="8"/>
+      <c r="A246" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B246" s="78"/>
+      <c r="C246" s="79"/>
+      <c r="D246" s="79"/>
+      <c r="E246" s="79"/>
+      <c r="F246" s="79"/>
+      <c r="G246" s="80"/>
     </row>
     <row r="247" spans="1:7">
       <c r="A247" s="8"/>
@@ -11150,7 +11127,7 @@
       <c r="F438" s="8"/>
       <c r="G438" s="8"/>
     </row>
-    <row r="439" spans="1:8">
+    <row r="439" spans="1:8" s="35" customFormat="1">
       <c r="A439" s="8"/>
       <c r="B439" s="8"/>
       <c r="C439" s="8"/>
@@ -11158,6 +11135,7 @@
       <c r="E439" s="8"/>
       <c r="F439" s="8"/>
       <c r="G439" s="8"/>
+      <c r="H439" s="12"/>
     </row>
     <row r="440" spans="1:8" s="35" customFormat="1">
       <c r="A440" s="8"/>
@@ -11209,14 +11187,13 @@
       <c r="G444" s="8"/>
       <c r="H444" s="12"/>
     </row>
-    <row r="445" spans="1:8" s="35" customFormat="1">
-      <c r="A445" s="8"/>
-      <c r="B445" s="8"/>
-      <c r="C445" s="8"/>
-      <c r="D445" s="8"/>
-      <c r="E445" s="8"/>
-      <c r="F445" s="8"/>
-      <c r="G445" s="8"/>
+    <row r="445" spans="1:8" s="35" customFormat="1" ht="15.75">
+      <c r="A445" s="15"/>
+      <c r="B445" s="34"/>
+      <c r="C445" s="34"/>
+      <c r="D445" s="55"/>
+      <c r="E445" s="56"/>
+      <c r="F445" s="57"/>
       <c r="H445" s="12"/>
     </row>
     <row r="446" spans="1:8" s="35" customFormat="1" ht="15.75">
@@ -15791,14 +15768,13 @@
       <c r="F953" s="57"/>
       <c r="H953" s="12"/>
     </row>
-    <row r="954" spans="1:8" s="35" customFormat="1" ht="15.75">
+    <row r="954" spans="1:8" ht="15.75">
       <c r="A954" s="15"/>
       <c r="B954" s="34"/>
       <c r="C954" s="34"/>
       <c r="D954" s="55"/>
       <c r="E954" s="56"/>
       <c r="F954" s="57"/>
-      <c r="H954" s="12"/>
     </row>
     <row r="955" spans="1:8" ht="15.75">
       <c r="A955" s="15"/>
@@ -15864,78 +15840,11 @@
       <c r="E962" s="56"/>
       <c r="F962" s="57"/>
     </row>
-    <row r="963" spans="1:6" ht="15.75">
-      <c r="A963" s="15"/>
-      <c r="B963" s="34"/>
-      <c r="C963" s="34"/>
-      <c r="D963" s="55"/>
-      <c r="E963" s="56"/>
-      <c r="F963" s="57"/>
-    </row>
   </sheetData>
-  <mergeCells count="87">
-    <mergeCell ref="B239:G239"/>
-    <mergeCell ref="B223:G223"/>
-    <mergeCell ref="B224:E224"/>
-    <mergeCell ref="B225:G225"/>
-    <mergeCell ref="B231:G231"/>
-    <mergeCell ref="B232:E232"/>
-    <mergeCell ref="B209:G209"/>
-    <mergeCell ref="B215:G215"/>
-    <mergeCell ref="B216:E216"/>
-    <mergeCell ref="B217:G217"/>
-    <mergeCell ref="B233:G233"/>
-    <mergeCell ref="B199:G199"/>
-    <mergeCell ref="B200:E200"/>
-    <mergeCell ref="B201:G201"/>
-    <mergeCell ref="B207:G207"/>
-    <mergeCell ref="B208:E208"/>
-    <mergeCell ref="B184:E184"/>
-    <mergeCell ref="B185:G185"/>
-    <mergeCell ref="B191:G191"/>
-    <mergeCell ref="B192:E192"/>
-    <mergeCell ref="B193:G193"/>
-    <mergeCell ref="B169:G169"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="B177:G177"/>
-    <mergeCell ref="B183:G183"/>
-    <mergeCell ref="B159:G159"/>
-    <mergeCell ref="B160:E160"/>
-    <mergeCell ref="B161:G161"/>
-    <mergeCell ref="B167:G167"/>
-    <mergeCell ref="B168:E168"/>
-    <mergeCell ref="B144:E144"/>
-    <mergeCell ref="B145:G145"/>
-    <mergeCell ref="B152:G152"/>
-    <mergeCell ref="B153:E153"/>
-    <mergeCell ref="B154:G154"/>
-    <mergeCell ref="B129:G129"/>
-    <mergeCell ref="B135:G135"/>
-    <mergeCell ref="B136:E136"/>
-    <mergeCell ref="B137:G137"/>
-    <mergeCell ref="B143:G143"/>
-    <mergeCell ref="B119:G119"/>
-    <mergeCell ref="B120:E120"/>
-    <mergeCell ref="B121:G121"/>
-    <mergeCell ref="B127:G127"/>
-    <mergeCell ref="B128:E128"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B105:G105"/>
-    <mergeCell ref="B111:G111"/>
-    <mergeCell ref="B112:E112"/>
-    <mergeCell ref="B113:G113"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="B65:G65"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B81:G81"/>
-    <mergeCell ref="B103:G103"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
+  <mergeCells count="90">
+    <mergeCell ref="B240:E240"/>
+    <mergeCell ref="B241:G241"/>
+    <mergeCell ref="B246:G246"/>
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:E24"/>
@@ -15950,6 +15859,17 @@
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B45:G45"/>
     <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B65:G65"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B81:G81"/>
+    <mergeCell ref="B103:G103"/>
     <mergeCell ref="B93:G93"/>
     <mergeCell ref="B58:E58"/>
     <mergeCell ref="B59:G59"/>
@@ -15961,9 +15881,60 @@
     <mergeCell ref="B83:G83"/>
     <mergeCell ref="B92:E92"/>
     <mergeCell ref="B91:G91"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B105:G105"/>
+    <mergeCell ref="B111:G111"/>
+    <mergeCell ref="B112:E112"/>
+    <mergeCell ref="B113:G113"/>
+    <mergeCell ref="B119:G119"/>
+    <mergeCell ref="B120:E120"/>
+    <mergeCell ref="B121:G121"/>
+    <mergeCell ref="B127:G127"/>
+    <mergeCell ref="B128:E128"/>
+    <mergeCell ref="B129:G129"/>
+    <mergeCell ref="B135:G135"/>
+    <mergeCell ref="B136:E136"/>
+    <mergeCell ref="B137:G137"/>
+    <mergeCell ref="B143:G143"/>
+    <mergeCell ref="B144:E144"/>
+    <mergeCell ref="B145:G145"/>
+    <mergeCell ref="B152:G152"/>
+    <mergeCell ref="B153:E153"/>
+    <mergeCell ref="B154:G154"/>
+    <mergeCell ref="B159:G159"/>
+    <mergeCell ref="B160:E160"/>
+    <mergeCell ref="B161:G161"/>
+    <mergeCell ref="B167:G167"/>
+    <mergeCell ref="B168:E168"/>
+    <mergeCell ref="B169:G169"/>
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B176:E176"/>
+    <mergeCell ref="B177:G177"/>
+    <mergeCell ref="B183:G183"/>
+    <mergeCell ref="B184:E184"/>
+    <mergeCell ref="B185:G185"/>
+    <mergeCell ref="B191:G191"/>
+    <mergeCell ref="B192:E192"/>
+    <mergeCell ref="B193:G193"/>
+    <mergeCell ref="B199:G199"/>
+    <mergeCell ref="B200:E200"/>
+    <mergeCell ref="B201:G201"/>
+    <mergeCell ref="B207:G207"/>
+    <mergeCell ref="B208:E208"/>
+    <mergeCell ref="B209:G209"/>
+    <mergeCell ref="B215:G215"/>
+    <mergeCell ref="B216:E216"/>
+    <mergeCell ref="B217:G217"/>
+    <mergeCell ref="B233:G233"/>
+    <mergeCell ref="B239:G239"/>
+    <mergeCell ref="B223:G223"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="B225:G225"/>
+    <mergeCell ref="B231:G231"/>
+    <mergeCell ref="B232:E232"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F446:F448 F453:F459 F672:F674 F662:F667 F464:F473 F478:F481 F486:F491 F496:F504 F509:F518 F523:F533 F538:F548 F564:F570 F592:F594 F553:F559 F575:F581 F586:F587 F599:F605 F610:F616 F632:F634 F621:F627 F639:F642 F647:F649 F654:F657 F21:F22 F76:F78 F85:F87 F95:F97 F235:F238 F35:F37 F42:F44 F49:F50 F55:F56 F61:F64 F69:F71 F107:F109 F115:F117 F123:F125 F131:F133 F139:F141 F147:F149 F156:F158 F163:F166 F171:F174 F179:F182 F187:F190 F195:F198 F203:F206 F211:F214 F219:F222 F227:F230 F27:F30" xr:uid="{04BF5218-6E63-4791-8319-1BD8E8E2885B}">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F445:F447 F452:F458 F671:F673 F661:F666 F463:F472 F477:F480 F485:F490 F495:F503 F508:F517 F522:F532 F537:F547 F563:F569 F591:F593 F552:F558 F574:F580 F585:F586 F598:F604 F609:F615 F631:F633 F620:F626 F638:F641 F646:F648 F653:F656 F243:F245 F27:F30 F227:F230 F219:F222 F211:F214 F203:F206 F195:F198 F187:F190 F179:F182 F171:F174 F163:F166 F156:F158 F147:F149 F139:F141 F131:F133 F123:F125 F115:F117 F107:F109 F69:F71 F61:F64 F55:F56 F49:F50 F42:F44 F35:F37 F235:F238 F95:F97 F85:F87 F76:F78 F21:F22">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>